<commit_message>
- removed DIR from the script and reverted back to T: for the default directory. Need to clean this up later  - Copied the 10_24_24 version of the AST tool (formally known as beta) to the working directory and redirected the sys.path.append to that folder. Tested and working  - Removed a redundant "Dont overwrite outputs" to True from Add Jobs, kept the one is re Load jobs
</commit_message>
<xml_diff>
--- a/autoast/4_jobs_tested.xlsx
+++ b/autoast/4_jobs_tested.xlsx
@@ -691,7 +691,7 @@
       </c>
       <c r="M2" s="13" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="N2" s="7" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="M3" s="13" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="N3" s="10" t="inlineStr">

</xml_diff>